<commit_message>
misc clean up and adding race-ethnicity
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/Year to Year-Group Linkage.xlsx
+++ b/myCBD/myInfo/Year to Year-Group Linkage.xlsx
@@ -14,12 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="12">
   <si>
     <t>year</t>
-  </si>
-  <si>
-    <t>yGroup1</t>
   </si>
   <si>
     <t>2013-2017</t>
@@ -33,12 +30,33 @@
   <si>
     <t>2000-2002</t>
   </si>
+  <si>
+    <t>yearGroup3</t>
+  </si>
+  <si>
+    <t>2015-2017</t>
+  </si>
+  <si>
+    <t>2012-2014</t>
+  </si>
+  <si>
+    <t>2009-2011</t>
+  </si>
+  <si>
+    <t>2006-2008</t>
+  </si>
+  <si>
+    <t>2003-2005</t>
+  </si>
+  <si>
+    <t>yearGroup5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -185,6 +203,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -530,10 +554,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -881,180 +915,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="14" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>2000</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <f>A2+1</f>
         <v>2001</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <f t="shared" ref="A4:A18" si="0">A3+1</f>
         <v>2002</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
       </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
       </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
       </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
       </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
       </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
       </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
       </c>
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
       </c>
-      <c r="B18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
         <v>2017</v>
       </c>
-      <c r="B19" t="s">
-        <v>2</v>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addition of 2018 death data, addition of 5-year county aggregation, other minor edits
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/Year to Year-Group Linkage.xlsx
+++ b/myCBD/myInfo/Year to Year-Group Linkage.xlsx
@@ -14,45 +14,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
   <si>
     <t>year</t>
   </si>
   <si>
-    <t>2013-2017</t>
-  </si>
-  <si>
-    <t>2008-2012</t>
-  </si>
-  <si>
-    <t>2003-2007</t>
-  </si>
-  <si>
-    <t>2000-2002</t>
-  </si>
-  <si>
     <t>yearGroup3</t>
   </si>
   <si>
-    <t>2015-2017</t>
-  </si>
-  <si>
-    <t>2012-2014</t>
-  </si>
-  <si>
-    <t>2009-2011</t>
-  </si>
-  <si>
-    <t>2006-2008</t>
-  </si>
-  <si>
-    <t>2003-2005</t>
-  </si>
-  <si>
     <t>yearGroup5</t>
   </si>
   <si>
-    <t>midYear</t>
+    <t>2014-2018</t>
+  </si>
+  <si>
+    <t>2009-2013</t>
+  </si>
+  <si>
+    <t>2000-2003</t>
+  </si>
+  <si>
+    <t>2004-2008</t>
+  </si>
+  <si>
+    <t>2016-2018</t>
+  </si>
+  <si>
+    <t>2013-2015</t>
+  </si>
+  <si>
+    <t>2010-2012</t>
+  </si>
+  <si>
+    <t>2007-2009</t>
+  </si>
+  <si>
+    <t>2004-2006</t>
+  </si>
+  <si>
+    <t>2001-2003</t>
+  </si>
+  <si>
+    <t>2000-2000</t>
+  </si>
+  <si>
+    <t>midYear3</t>
+  </si>
+  <si>
+    <t>midYear5</t>
   </si>
 </sst>
 </file>
@@ -919,299 +928,362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="14" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="14" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>2000</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <f>A2+1</f>
         <v>2001</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A18" si="0">A3+1</f>
         <v>2002</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <f t="shared" si="0"/>
+        <v>2003</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <f t="shared" si="0"/>
+        <v>2004</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2006</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <f t="shared" si="0"/>
+        <v>2005</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2006</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <f t="shared" si="0"/>
+        <v>2006</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2006</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <f t="shared" si="0"/>
+        <v>2007</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2006</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <f t="shared" si="0"/>
+        <v>2008</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2006</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <f t="shared" si="0"/>
+        <v>2009</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C11" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <f t="shared" si="0"/>
+        <v>2010</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <f t="shared" si="0"/>
-        <v>2003</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="C12" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <f t="shared" si="0"/>
-        <v>2004</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="C16" s="2">
+        <v>2016</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <f t="shared" si="0"/>
+        <v>2015</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <f t="shared" si="0"/>
-        <v>2005</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="C17" s="2">
+        <v>2016</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <f t="shared" si="0"/>
-        <v>2006</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <f t="shared" si="0"/>
-        <v>2007</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <f t="shared" si="0"/>
-        <v>2008</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <f t="shared" si="0"/>
-        <v>2009</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <f t="shared" si="0"/>
-        <v>2010</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <f t="shared" si="0"/>
-        <v>2011</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <f t="shared" si="0"/>
-        <v>2012</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="C18" s="2">
+        <v>2016</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D14">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <f t="shared" si="0"/>
-        <v>2013</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <f t="shared" si="0"/>
-        <v>2014</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <f t="shared" si="0"/>
-        <v>2015</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>2017</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2">
         <v>2016</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2016</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>2017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating for 2019 (and 2020)
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/Year to Year-Group Linkage.xlsx
+++ b/myCBD/myInfo/Year to Year-Group Linkage.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CCB\CCB Project\0.CCB\myCBD\myInfo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="9" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="17">
   <si>
     <t>year</t>
   </si>
@@ -25,49 +31,52 @@
     <t>yearGroup5</t>
   </si>
   <si>
-    <t>2014-2018</t>
-  </si>
-  <si>
-    <t>2009-2013</t>
-  </si>
-  <si>
-    <t>2000-2003</t>
-  </si>
-  <si>
-    <t>2004-2008</t>
-  </si>
-  <si>
-    <t>2016-2018</t>
-  </si>
-  <si>
-    <t>2013-2015</t>
-  </si>
-  <si>
-    <t>2010-2012</t>
-  </si>
-  <si>
-    <t>2007-2009</t>
-  </si>
-  <si>
-    <t>2004-2006</t>
-  </si>
-  <si>
-    <t>2001-2003</t>
-  </si>
-  <si>
-    <t>2000-2000</t>
-  </si>
-  <si>
     <t>midYear3</t>
   </si>
   <si>
     <t>midYear5</t>
+  </si>
+  <si>
+    <t>2015-2019</t>
+  </si>
+  <si>
+    <t>2010-2014</t>
+  </si>
+  <si>
+    <t>2005-2009</t>
+  </si>
+  <si>
+    <t>2000-2004</t>
+  </si>
+  <si>
+    <t>2017-2019</t>
+  </si>
+  <si>
+    <t>2014-2016</t>
+  </si>
+  <si>
+    <t>2011-2013</t>
+  </si>
+  <si>
+    <t>2008-2010</t>
+  </si>
+  <si>
+    <t>2005-2007</t>
+  </si>
+  <si>
+    <t>2002-2004</t>
+  </si>
+  <si>
+    <t>2000-2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -684,7 +693,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -719,7 +728,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -928,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -949,13 +958,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -963,11 +972,13 @@
         <v>2000</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2002</v>
+      </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -976,14 +987,16 @@
         <v>2001</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2002</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>2002</v>
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -992,14 +1005,16 @@
         <v>2002</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2002</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E4">
-        <v>2002</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1008,14 +1023,16 @@
         <v>2003</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2002</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5">
-        <v>2002</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1024,16 +1041,16 @@
         <v>2004</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
-        <v>2006</v>
+        <v>2002</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E6">
-        <v>2005</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1041,17 +1058,17 @@
         <f t="shared" si="0"/>
         <v>2005</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C7" s="3">
+        <v>2007</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7">
         <v>2006</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7">
-        <v>2005</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1059,17 +1076,17 @@
         <f t="shared" si="0"/>
         <v>2006</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C8" s="3">
+        <v>2007</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8">
         <v>2006</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8">
-        <v>2005</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1077,17 +1094,17 @@
         <f t="shared" si="0"/>
         <v>2007</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>6</v>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C9" s="3">
+        <v>2007</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9">
         <v>2006</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <v>2008</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1095,17 +1112,17 @@
         <f t="shared" si="0"/>
         <v>2008</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>6</v>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C10" s="3">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E10">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1114,16 +1131,16 @@
         <v>2009</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2">
-        <v>2011</v>
+        <v>7</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2007</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E11">
-        <v>2008</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1132,16 +1149,16 @@
         <v>2010</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E12">
-        <v>2011</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1150,16 +1167,16 @@
         <v>2011</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E13">
-        <v>2011</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1168,16 +1185,16 @@
         <v>2012</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C14" s="2">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E14">
-        <v>2011</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1186,16 +1203,16 @@
         <v>2013</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E15">
-        <v>2014</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1204,16 +1221,16 @@
         <v>2014</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C16" s="2">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E16">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1222,16 +1239,16 @@
         <v>2015</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C17" s="2">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E17">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1240,16 +1257,16 @@
         <v>2016</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C18" s="2">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E18">
-        <v>2017</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1257,16 +1274,16 @@
         <v>2017</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C19" s="2">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E19">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1274,20 +1291,49 @@
         <v>2018</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C20" s="2">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E20">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2">
         <v>2017</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>